<commit_message>
Washignton water right update 11302020.
Washignton water right update 11302020.
</commit_message>
<xml_diff>
--- a/Washington/WaterAllocation/WA_Allocation Schema Mapping_WaDEQA.xlsx
+++ b/Washington/WaterAllocation/WA_Allocation Schema Mapping_WaDEQA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\State Mapping Projects\WA Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Washington\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE46E65-7AE0-4A01-8448-62EE96559A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3363BC-9099-4718-BC71-58A789287EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="336">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -1062,27 +1062,6 @@
   </si>
   <si>
     <t>1) Joined PoD data -to- bridge table -to- Use and Person data.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Geographic Water Information System (GWIS)Data from the WA stat: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://fortress.wa.gov/ecy/gispublic/DataDownload/wr/GWIS_Data/</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1131,6 +1110,30 @@
   </si>
   <si>
     <t>3) Some WRs had too many sites and had to be removed (see allocations_missing).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Geographic Water Information System (GWIS) Data from the WA state: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://fortress.wa.gov/ecy/gispublic/DataDownload/wr/GWIS_Data/</t>
+    </r>
+  </si>
+  <si>
+    <t>4) Input data has roughly 74,184 duplicate rows.  Need to ask MT if that is suppose to happen or if it was by accident.</t>
   </si>
 </sst>
 </file>
@@ -2527,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2560,17 +2563,17 @@
         <v>244</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="92" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" s="92" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2586,12 +2589,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>